<commit_message>
update chart code; metrics analysis
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -390,13 +390,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>41.87</v>
+        <v>41.88</v>
       </c>
       <c r="C2" t="n">
         <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3">
@@ -404,13 +404,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>17.85</v>
+        <v>24.46</v>
       </c>
       <c r="C3" t="n">
-        <v>4.17</v>
+        <v>14.58</v>
       </c>
       <c r="D3" t="n">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -469,13 +469,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>68.52</v>
+        <v>68.88</v>
       </c>
       <c r="D3" t="n">
         <v>80</v>
       </c>
       <c r="E3" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
@@ -486,13 +486,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>6.32</v>
+        <v>14.18</v>
       </c>
       <c r="D4" t="n">
-        <v>4.17</v>
+        <v>14.58</v>
       </c>
       <c r="E4" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
@@ -503,13 +503,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>48.89</v>
+        <v>51.9</v>
       </c>
       <c r="D5" t="n">
         <v>50</v>
       </c>
       <c r="E5" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>